<commit_message>
Add version number in readme
</commit_message>
<xml_diff>
--- a/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_templates/MIAPPEv1.1_training_spreadsheet.xlsx
+++ b/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_templates/MIAPPEv1.1_training_spreadsheet.xlsx
@@ -33,9 +33,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="553">
   <si>
     <t xml:space="preserve">README</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIAPPE Version 1.2</t>
   </si>
   <si>
     <t xml:space="preserve">Here are described the different sheets of this template and their respective fields.</t>
@@ -2449,7 +2452,9 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -2481,7 +2486,7 @@
     </row>
     <row r="2" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -2515,7 +2520,7 @@
     </row>
     <row r="3" s="9" customFormat="true" ht="84.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -2549,7 +2554,7 @@
     </row>
     <row r="4" customFormat="false" ht="69.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
@@ -2573,7 +2578,7 @@
     </row>
     <row r="5" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -2597,31 +2602,31 @@
     </row>
     <row r="6" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J6" s="18"/>
       <c r="K6" s="18"/>
@@ -2637,31 +2642,31 @@
     </row>
     <row r="7" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J7" s="21"/>
       <c r="K7" s="21"/>
@@ -2677,31 +2682,31 @@
     </row>
     <row r="8" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" s="23" t="n">
         <v>41260</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J8" s="21"/>
       <c r="K8" s="21"/>
@@ -2717,31 +2722,31 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>32</v>
-      </c>
       <c r="H9" s="22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J9" s="21"/>
       <c r="K9" s="21"/>
@@ -2757,7 +2762,7 @@
     </row>
     <row r="10" customFormat="false" ht="69.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -2781,7 +2786,7 @@
     </row>
     <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
@@ -2805,255 +2810,255 @@
     </row>
     <row r="12" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M12" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N12" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="O12" s="16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P12" s="17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Q12" s="17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="R12" s="16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="S12" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T12" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J13" s="22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L13" s="22" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M13" s="22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="N13" s="22" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O13" s="22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="P13" s="22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="Q13" s="22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="R13" s="22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="S13" s="25" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="T13" s="22" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F14" s="23" t="n">
         <v>37587</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J14" s="20" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K14" s="20" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L14" s="20" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M14" s="20" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="N14" s="22" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="O14" s="22" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="P14" s="22" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="Q14" s="22" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="R14" s="22" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="S14" s="25" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="T14" s="26" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D15" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="H15" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="I15" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K15" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="L15" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="M15" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="N15" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="O15" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="P15" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="I15" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="J15" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="K15" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="L15" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="M15" s="22" t="s">
+      <c r="Q15" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="N15" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="O15" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="P15" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q15" s="22" t="s">
-        <v>33</v>
-      </c>
       <c r="R15" s="22" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="S15" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="T15" s="22" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="69.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
@@ -3077,7 +3082,7 @@
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
@@ -3101,25 +3106,25 @@
     </row>
     <row r="18" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
@@ -3137,25 +3142,25 @@
     </row>
     <row r="19" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G19" s="22" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
@@ -3173,25 +3178,25 @@
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
@@ -3209,25 +3214,25 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F21" s="22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G21" s="22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
@@ -3245,7 +3250,7 @@
     </row>
     <row r="22" customFormat="false" ht="69.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
@@ -3269,7 +3274,7 @@
     </row>
     <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="14" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
@@ -3293,19 +3298,19 @@
     </row>
     <row r="24" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F24" s="27"/>
       <c r="G24" s="27"/>
@@ -3325,19 +3330,19 @@
     </row>
     <row r="25" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
@@ -3357,19 +3362,19 @@
     </row>
     <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
@@ -3389,19 +3394,19 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
@@ -3421,7 +3426,7 @@
     </row>
     <row r="28" customFormat="false" ht="69.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -3445,7 +3450,7 @@
     </row>
     <row r="29" customFormat="false" ht="69.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="14" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -3469,247 +3474,247 @@
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I30" s="16" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J30" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K30" s="16" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="L30" s="16" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="M30" s="16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="N30" s="16" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="O30" s="16" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="P30" s="16" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="Q30" s="16" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="R30" s="16" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="S30" s="16" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="T30" s="13"/>
     </row>
     <row r="31" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F31" s="22" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G31" s="22" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H31" s="22" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I31" s="22" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J31" s="22" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="K31" s="22" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="L31" s="22" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="M31" s="22" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="N31" s="22" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="O31" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="P31" s="22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="Q31" s="22" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="R31" s="22" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="S31" s="22" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="T31" s="13"/>
     </row>
     <row r="32" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H32" s="20" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="I32" s="20" t="n">
         <v>-8.73</v>
       </c>
       <c r="J32" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="K32" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="L32" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="M32" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="N32" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="O32" s="20" t="s">
         <v>182</v>
-      </c>
-      <c r="K32" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="L32" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="M32" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="N32" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="O32" s="20" t="s">
-        <v>181</v>
       </c>
       <c r="P32" s="20" t="n">
         <v>-8.73</v>
       </c>
       <c r="Q32" s="20" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="R32" s="22" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="S32" s="22" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="T32" s="13"/>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F33" s="22" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G33" s="22" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H33" s="22" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I33" s="22" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J33" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="K33" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="L33" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="M33" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="N33" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="O33" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="K33" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="L33" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="M33" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="N33" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="O33" s="22" t="s">
-        <v>97</v>
-      </c>
       <c r="P33" s="22" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Q33" s="22" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="R33" s="22" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="S33" s="22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="T33" s="13"/>
     </row>
     <row r="34" customFormat="false" ht="69.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="11" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
@@ -3733,7 +3738,7 @@
     </row>
     <row r="35" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="14" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
@@ -3757,16 +3762,16 @@
     </row>
     <row r="36" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
@@ -3787,16 +3792,16 @@
     </row>
     <row r="37" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E37" s="13"/>
       <c r="F37" s="13"/>
@@ -3817,16 +3822,16 @@
     </row>
     <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
@@ -3847,16 +3852,16 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E39" s="28"/>
       <c r="F39" s="13"/>
@@ -3877,7 +3882,7 @@
     </row>
     <row r="40" customFormat="false" ht="69.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
@@ -3901,7 +3906,7 @@
     </row>
     <row r="41" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="14" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
@@ -3925,19 +3930,19 @@
     </row>
     <row r="42" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F42" s="13"/>
       <c r="G42" s="13"/>
@@ -3957,19 +3962,19 @@
     </row>
     <row r="43" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D43" s="29" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E43" s="29" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F43" s="30"/>
       <c r="G43" s="30"/>
@@ -3989,19 +3994,19 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D44" s="29" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F44" s="30"/>
       <c r="G44" s="30"/>
@@ -4021,19 +4026,19 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C45" s="29" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D45" s="29" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F45" s="30"/>
       <c r="G45" s="30"/>
@@ -4053,7 +4058,7 @@
     </row>
     <row r="46" customFormat="false" ht="69.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="11" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
@@ -4077,7 +4082,7 @@
     </row>
     <row r="47" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="14" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
@@ -4101,25 +4106,25 @@
     </row>
     <row r="48" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F48" s="16" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G48" s="17" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H48" s="31"/>
       <c r="I48" s="31"/>
@@ -4137,25 +4142,25 @@
     </row>
     <row r="49" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F49" s="22" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G49" s="22" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H49" s="30"/>
       <c r="I49" s="30"/>
@@ -4173,25 +4178,25 @@
     </row>
     <row r="50" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D50" s="22" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E50" s="22" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F50" s="22" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G50" s="22" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H50" s="30"/>
       <c r="I50" s="30"/>
@@ -4209,25 +4214,25 @@
     </row>
     <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B51" s="22" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F51" s="22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G51" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H51" s="30"/>
       <c r="I51" s="30"/>
@@ -4245,7 +4250,7 @@
     </row>
     <row r="52" customFormat="false" ht="69.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="11" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
@@ -4269,7 +4274,7 @@
     </row>
     <row r="53" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="14" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
@@ -4293,28 +4298,28 @@
     </row>
     <row r="54" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E54" s="17" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F54" s="16" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="G54" s="16" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H54" s="16" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="I54" s="31"/>
       <c r="J54" s="31"/>
@@ -4331,28 +4336,28 @@
     </row>
     <row r="55" customFormat="false" ht="147.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D55" s="29" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E55" s="29" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F55" s="29" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G55" s="29" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="H55" s="29" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="I55" s="32"/>
       <c r="J55" s="32"/>
@@ -4369,28 +4374,28 @@
     </row>
     <row r="56" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D56" s="29" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E56" s="29" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F56" s="29" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="G56" s="29" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H56" s="29" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="I56" s="32"/>
       <c r="J56" s="32"/>
@@ -4407,28 +4412,28 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B57" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D57" s="29" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E57" s="29" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F57" s="29" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G57" s="29" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H57" s="29" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I57" s="32"/>
       <c r="J57" s="32"/>
@@ -4445,7 +4450,7 @@
     </row>
     <row r="58" customFormat="false" ht="69.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="11" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B58" s="12"/>
       <c r="C58" s="12"/>
@@ -4469,7 +4474,7 @@
     </row>
     <row r="59" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="14" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
@@ -4493,28 +4498,28 @@
     </row>
     <row r="60" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D60" s="16" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E60" s="17" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F60" s="16" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="G60" s="17" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="H60" s="16" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="I60" s="33"/>
       <c r="J60" s="33"/>
@@ -4531,28 +4536,28 @@
     </row>
     <row r="61" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E61" s="22" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F61" s="22" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G61" s="22" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="H61" s="22" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="I61" s="34"/>
       <c r="J61" s="34"/>
@@ -4569,28 +4574,28 @@
     </row>
     <row r="62" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E62" s="22" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F62" s="22" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G62" s="22" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="H62" s="22" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="I62" s="34"/>
       <c r="J62" s="34"/>
@@ -4607,28 +4612,28 @@
     </row>
     <row r="63" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C63" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E63" s="22" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F63" s="22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G63" s="22" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="H63" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I63" s="34"/>
       <c r="J63" s="34"/>
@@ -4645,7 +4650,7 @@
     </row>
     <row r="64" customFormat="false" ht="69.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="11" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B64" s="12"/>
       <c r="C64" s="12"/>
@@ -4669,7 +4674,7 @@
     </row>
     <row r="65" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="14" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="12"/>
@@ -4693,46 +4698,46 @@
     </row>
     <row r="66" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E66" s="16" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F66" s="17" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="G66" s="16" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="H66" s="17" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="I66" s="16" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J66" s="16" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="K66" s="16" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="L66" s="17" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="M66" s="16" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="N66" s="16" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="O66" s="13"/>
       <c r="P66" s="13"/>
@@ -4743,46 +4748,46 @@
     </row>
     <row r="67" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="35" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B67" s="22" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C67" s="22" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D67" s="22" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E67" s="22" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F67" s="22" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G67" s="22" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="H67" s="22" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="I67" s="22" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="J67" s="22" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="K67" s="22" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="L67" s="22" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="M67" s="22" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="N67" s="22" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="O67" s="13"/>
       <c r="P67" s="13"/>
@@ -4793,46 +4798,46 @@
     </row>
     <row r="68" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="35" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B68" s="22" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C68" s="22" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D68" s="22" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E68" s="22" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="F68" s="22" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G68" s="22" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="H68" s="22" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="I68" s="22" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="J68" s="22" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="K68" s="36" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="L68" s="22" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="M68" s="22" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="N68" s="22" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="O68" s="13"/>
       <c r="P68" s="13"/>
@@ -4843,46 +4848,46 @@
     </row>
     <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B69" s="22" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C69" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D69" s="22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E69" s="22" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="F69" s="22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G69" s="22" t="s">
+        <v>320</v>
+      </c>
+      <c r="H69" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="I69" s="22" t="s">
+        <v>320</v>
+      </c>
+      <c r="J69" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="K69" s="22" t="s">
+        <v>321</v>
+      </c>
+      <c r="L69" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="M69" s="22" t="s">
         <v>319</v>
       </c>
-      <c r="H69" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="I69" s="22" t="s">
-        <v>319</v>
-      </c>
-      <c r="J69" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="K69" s="22" t="s">
-        <v>320</v>
-      </c>
-      <c r="L69" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="M69" s="22" t="s">
-        <v>318</v>
-      </c>
       <c r="N69" s="22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O69" s="13"/>
       <c r="P69" s="13"/>
@@ -4893,7 +4898,7 @@
     </row>
     <row r="70" customFormat="false" ht="69.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="11" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B70" s="12"/>
       <c r="C70" s="12"/>
@@ -4917,7 +4922,7 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="37" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B71" s="12"/>
       <c r="C71" s="12"/>
@@ -4941,7 +4946,7 @@
     </row>
     <row r="72" customFormat="false" ht="69.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="11" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B72" s="12"/>
       <c r="C72" s="12"/>
@@ -4965,7 +4970,7 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="6" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B73" s="12"/>
       <c r="C73" s="12"/>
@@ -5919,25 +5924,25 @@
   <sheetData>
     <row r="1" s="41" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="H1" s="45"/>
       <c r="I1" s="45"/>
@@ -7089,25 +7094,25 @@
   <sheetData>
     <row r="1" s="41" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H1" s="33"/>
       <c r="I1" s="33"/>
@@ -8259,43 +8264,43 @@
   <sheetData>
     <row r="1" s="41" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="L1" s="16" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="N1" s="46"/>
       <c r="O1" s="46"/>
@@ -9438,7 +9443,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -9462,7 +9467,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -9508,21 +9513,21 @@
     </row>
     <row r="4" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="49" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="49" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B5" s="50"/>
       <c r="C5" s="50"/>
@@ -9530,273 +9535,273 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="51" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C6" s="51" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D6" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="51" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C7" s="51" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D7" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="51" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C8" s="51" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D8" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="51" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B9" s="51" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C9" s="51" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D9" s="51" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="51" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C10" s="51" t="n">
         <v>16</v>
       </c>
       <c r="D10" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="51" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C11" s="51" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D11" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="51" t="s">
+        <v>348</v>
+      </c>
+      <c r="B12" s="51" t="s">
+        <v>349</v>
+      </c>
+      <c r="C12" s="51" t="s">
         <v>347</v>
       </c>
-      <c r="B12" s="51" t="s">
-        <v>348</v>
-      </c>
-      <c r="C12" s="51" t="s">
-        <v>346</v>
-      </c>
       <c r="D12" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="51" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C13" s="51" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D13" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="51" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C14" s="51" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D14" s="51" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="51" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C15" s="51" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D15" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="51" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C16" s="51" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D16" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="51" t="s">
+        <v>362</v>
+      </c>
+      <c r="B17" s="51" t="s">
+        <v>363</v>
+      </c>
+      <c r="C17" s="51" t="s">
         <v>361</v>
       </c>
-      <c r="B17" s="51" t="s">
-        <v>362</v>
-      </c>
-      <c r="C17" s="51" t="s">
-        <v>360</v>
-      </c>
       <c r="D17" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="51" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C18" s="51" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D18" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="51" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D19" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="51" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B20" s="51" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C20" s="51" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="D20" s="51" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="51" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C21" s="51" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D21" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="51" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C22" s="51" t="n">
         <v>0.3</v>
       </c>
       <c r="D22" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="51" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B23" s="51" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C23" s="51" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D23" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="51" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B24" s="51" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C24" s="51" t="n">
         <v>0.33</v>
       </c>
       <c r="D24" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B25" s="50"/>
       <c r="C25" s="50"/>
@@ -9804,201 +9809,201 @@
     </row>
     <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="51" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B26" s="51" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C26" s="51" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D26" s="51" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="51" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C27" s="51" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D27" s="51" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="51" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B28" s="51" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C28" s="51" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D28" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="51" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C29" s="51" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D29" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="51" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B30" s="51" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C30" s="51" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D30" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="51" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B31" s="51" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C31" s="51" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D31" s="51" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="51" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B32" s="51" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C32" s="51" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D32" s="51" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B33" s="51" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C33" s="51"/>
       <c r="D33" s="51" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="51" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B34" s="51" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C34" s="51" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D34" s="51" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="51" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B35" s="51" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C35" s="51" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D35" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="51" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B36" s="51" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C36" s="51" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D36" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="51" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B37" s="51" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C37" s="51" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D37" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="51" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B38" s="51" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C38" s="51" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D38" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="51" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B39" s="51" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C39" s="51" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D39" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B40" s="50"/>
       <c r="C40" s="50"/>
@@ -10006,142 +10011,142 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="51" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B41" s="51" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C41" s="51" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D41" s="51" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="51" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B42" s="51" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C42" s="51" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="D42" s="51" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="51" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B43" s="51" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C43" s="51" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D43" s="51" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="51" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B44" s="51" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C44" s="51" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D44" s="51" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="51" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B45" s="51" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C45" s="51" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="D45" s="51" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="51" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B46" s="51" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C46" s="51" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D46" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="51" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B47" s="51" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C47" s="51" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D47" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="51" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B48" s="51" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C48" s="51" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D48" s="51" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="51" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B49" s="51" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C49" s="51" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D49" s="51" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="51" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B50" s="51" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C50" s="51" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D50" s="51" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -11129,7 +11134,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -11153,7 +11158,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -11199,362 +11204,362 @@
     </row>
     <row r="4" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="49" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="49" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="51" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C5" s="51" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D5" s="51" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="51" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C6" s="51" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="D6" s="51" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="51" t="s">
+        <v>466</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>467</v>
+      </c>
+      <c r="C7" s="51" t="s">
+        <v>468</v>
+      </c>
+      <c r="D7" s="51" t="s">
         <v>465</v>
-      </c>
-      <c r="B7" s="51" t="s">
-        <v>466</v>
-      </c>
-      <c r="C7" s="51" t="s">
-        <v>467</v>
-      </c>
-      <c r="D7" s="51" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="51" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C8" s="51" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D8" s="51" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="51" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B9" s="51" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C9" s="51" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="D9" s="51" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="51" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C10" s="51" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="D10" s="51" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="51" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C11" s="51" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="D11" s="51" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="51" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C12" s="51" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="D12" s="51" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="51" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C13" s="51" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="D13" s="51" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="51" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C14" s="51" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="D14" s="51" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="51" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C15" s="51" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="D15" s="51" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="51" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C16" s="51" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="D16" s="51" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="51" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C17" s="51" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D17" s="51" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="51" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C18" s="51" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="D18" s="51" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="51" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="D19" s="51" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="51" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B20" s="51" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C20" s="51" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="D20" s="51" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="51" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C21" s="51" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="D21" s="51" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="51" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="C22" s="51" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="D22" s="51" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="51" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B23" s="51" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C23" s="51" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="D23" s="51" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="51" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B24" s="51" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="C24" s="51" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="D24" s="51" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="51" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="B25" s="51" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="C25" s="51" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="D25" s="51" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="51" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B26" s="51" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="C26" s="51" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="D26" s="51" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="51" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="C27" s="51" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="D27" s="51" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="51" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B28" s="51" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C28" s="51" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="D28" s="51" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="51" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B29" s="51"/>
       <c r="C29" s="51"/>
       <c r="D29" s="51" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -12549,7 +12554,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12560,28 +12565,28 @@
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15623,61 +15628,61 @@
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="O1" s="17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q1" s="16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="R1" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S1" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16827,22 +16832,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17923,16 +17928,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E1" s="41"/>
       <c r="F1" s="41"/>
@@ -19021,58 +19026,58 @@
   <sheetData>
     <row r="1" s="41" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="L1" s="16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="P1" s="16" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="Q1" s="16" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="R1" s="16" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="S1" s="1"/>
     </row>
@@ -22217,13 +22222,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23284,16 +23289,16 @@
   <sheetData>
     <row r="1" s="41" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E1" s="43"/>
       <c r="F1" s="43"/>
@@ -24477,22 +24482,22 @@
   <sheetData>
     <row r="1" s="46" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G1" s="45"/>
       <c r="H1" s="45"/>

</xml_diff>